<commit_message>
Update README.md with notes
</commit_message>
<xml_diff>
--- a/coursera-DataDrivenTestExcel/testDataInputFiles/TestData.xlsx
+++ b/coursera-DataDrivenTestExcel/testDataInputFiles/TestData.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9A53EB6F-DB52-4B79-8465-F63A7CBDF9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alice\Documents\Development\TestAutomation\selenium-tutorials-java\coursera-DataDrivenTestExcel\testDataInputFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5A1C24-B156-4E67-8B35-890ECE18C57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +16,6 @@
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,16 +33,16 @@
     <t>mngr546830</t>
   </si>
   <si>
-    <t>bEhYrAs</t>
-  </si>
-  <si>
     <t>turAduz</t>
   </si>
   <si>
     <t>AsabEbY</t>
   </si>
   <si>
-    <t>mngr5460O3</t>
+    <t>mngr549847</t>
+  </si>
+  <si>
+    <t>surUpeg</t>
   </si>
 </sst>
 </file>
@@ -365,7 +369,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -375,10 +379,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -386,7 +390,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -394,7 +398,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>